<commit_message>
Add validation for formatting
</commit_message>
<xml_diff>
--- a/APACHE_POI/lib/src/main/resources/Activity.xlsx
+++ b/APACHE_POI/lib/src/main/resources/Activity.xlsx
@@ -2,17 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Country Population" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Flight Details" sheetId="2" r:id="rId5"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="42">
   <si>
     <t>Country</t>
   </si>
@@ -123,6 +125,21 @@
   </si>
   <si>
     <t>4h30m(Bengaluru)</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Jerusalem</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>24-02-2021</t>
+  </si>
+  <si>
+    <t>22145</t>
   </si>
 </sst>
 </file>
@@ -133,7 +150,7 @@
     <numFmt numFmtId="164" formatCode="dd-mm-yyyy"/>
     <numFmt numFmtId="165" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="23">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -160,8 +177,80 @@
       <color rgb="FF000000"/>
       <name val="Comic Sans MS"/>
     </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +263,36 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkDown">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkDown">
+        <bgColor indexed="3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkDown">
+        <bgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -181,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="62">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -206,6 +325,96 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -421,13 +630,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="25.5"/>
-    <col customWidth="1" min="6" max="6" width="23.63"/>
+    <col min="3" max="3" customWidth="true" width="25.5"/>
+    <col min="6" max="6" customWidth="true" width="23.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -440,7 +650,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="60" t="s">
         <v>3</v>
       </c>
     </row>
@@ -448,7 +658,7 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="59" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1">
@@ -498,6 +708,312 @@
       </c>
       <c r="D5" s="2">
         <v>44244.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="61" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -510,6 +1026,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>

</xml_diff>